<commit_message>
Added simple choice menu Separated program to different thread
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -531,10 +531,10 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>44.37</v>
+        <v>44.38</v>
       </c>
       <c r="J2" t="n">
-        <v>46.97</v>
+        <v>47</v>
       </c>
       <c r="K2" t="n">
         <v>88</v>
@@ -582,10 +582,10 @@
         <v>247</v>
       </c>
       <c r="I3" t="n">
-        <v>1095.91</v>
+        <v>1096.11</v>
       </c>
       <c r="J3" t="n">
-        <v>1160.04</v>
+        <v>1161</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
@@ -633,10 +633,10 @@
         <v>67</v>
       </c>
       <c r="I4" t="n">
-        <v>297.27</v>
+        <v>297.33</v>
       </c>
       <c r="J4" t="n">
-        <v>314.67</v>
+        <v>314.93</v>
       </c>
       <c r="K4" t="n">
         <v>12</v>
@@ -684,10 +684,10 @@
         <v>30</v>
       </c>
       <c r="I5" t="n">
-        <v>133.11</v>
+        <v>133.13</v>
       </c>
       <c r="J5" t="n">
-        <v>140.9</v>
+        <v>141.01</v>
       </c>
       <c r="K5" t="n">
         <v>701</v>
@@ -735,10 +735,10 @@
         <v>538</v>
       </c>
       <c r="I6" t="n">
-        <v>2387.05</v>
+        <v>2387.48</v>
       </c>
       <c r="J6" t="n">
-        <v>2526.72</v>
+        <v>2528.82</v>
       </c>
       <c r="K6" t="n">
         <v>83766</v>
@@ -786,10 +786,10 @@
         <v>140</v>
       </c>
       <c r="I7" t="n">
-        <v>621.17</v>
+        <v>621.28</v>
       </c>
       <c r="J7" t="n">
-        <v>657.51</v>
+        <v>658.0599999999999</v>
       </c>
       <c r="K7" t="n">
         <v>767</v>
@@ -837,10 +837,10 @@
         <v>270</v>
       </c>
       <c r="I8" t="n">
-        <v>1197.96</v>
+        <v>1198.18</v>
       </c>
       <c r="J8" t="n">
-        <v>1268.06</v>
+        <v>1269.11</v>
       </c>
       <c r="K8" t="n">
         <v>18</v>

</xml_diff>

<commit_message>
Added tests Refactored code to suit tests
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -531,10 +531,10 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>44.38</v>
+        <v>44.53</v>
       </c>
       <c r="J2" t="n">
-        <v>47</v>
+        <v>46.81</v>
       </c>
       <c r="K2" t="n">
         <v>88</v>
@@ -582,10 +582,10 @@
         <v>247</v>
       </c>
       <c r="I3" t="n">
-        <v>1096.11</v>
+        <v>1099.97</v>
       </c>
       <c r="J3" t="n">
-        <v>1161</v>
+        <v>1156.18</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
@@ -633,10 +633,10 @@
         <v>67</v>
       </c>
       <c r="I4" t="n">
-        <v>297.33</v>
+        <v>298.37</v>
       </c>
       <c r="J4" t="n">
-        <v>314.93</v>
+        <v>313.62</v>
       </c>
       <c r="K4" t="n">
         <v>12</v>
@@ -684,10 +684,10 @@
         <v>30</v>
       </c>
       <c r="I5" t="n">
-        <v>133.13</v>
+        <v>133.6</v>
       </c>
       <c r="J5" t="n">
-        <v>141.01</v>
+        <v>140.43</v>
       </c>
       <c r="K5" t="n">
         <v>701</v>
@@ -735,10 +735,10 @@
         <v>538</v>
       </c>
       <c r="I6" t="n">
-        <v>2387.48</v>
+        <v>2395.88</v>
       </c>
       <c r="J6" t="n">
-        <v>2528.82</v>
+        <v>2518.32</v>
       </c>
       <c r="K6" t="n">
         <v>83766</v>
@@ -786,10 +786,10 @@
         <v>140</v>
       </c>
       <c r="I7" t="n">
-        <v>621.28</v>
+        <v>623.46</v>
       </c>
       <c r="J7" t="n">
-        <v>658.0599999999999</v>
+        <v>655.33</v>
       </c>
       <c r="K7" t="n">
         <v>767</v>
@@ -837,10 +837,10 @@
         <v>270</v>
       </c>
       <c r="I8" t="n">
-        <v>1198.18</v>
+        <v>1202.39</v>
       </c>
       <c r="J8" t="n">
-        <v>1269.11</v>
+        <v>1263.84</v>
       </c>
       <c r="K8" t="n">
         <v>18</v>

</xml_diff>